<commit_message>
Slow but working GPU solver with reduction
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\CPDS\Paralelism\OpenMP\CPDS-M2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/be25f2d0b6efbae7/Documents/UPC/Semester 2/CPDS/Parallelism/CPDS-M2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3A80FB-3255-45BD-BDF5-7BB910E06272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{6B3A80FB-3255-45BD-BDF5-7BB910E06272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{22F03E9E-57B0-466A-AEC9-207FC503969F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A23B7361-40C4-4D57-8C04-7E547CDB9F70}"/>
+    <workbookView xWindow="-10326" yWindow="6558" windowWidth="17280" windowHeight="8994" xr2:uid="{A23B7361-40C4-4D57-8C04-7E547CDB9F70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,23 +77,29 @@
     <t>Original</t>
   </si>
   <si>
-    <t>V1 Time</t>
-  </si>
-  <si>
-    <t>V2 Time</t>
-  </si>
-  <si>
-    <t>V3 Time</t>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>GPU w/CPU reduc</t>
+  </si>
+  <si>
+    <t>GPU w/GPU reduc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -221,6 +227,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -230,14 +244,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,35 +565,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F57AE4-C9F8-44B0-9527-15A39F4715C1}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="9" max="9" width="14.9453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.20703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="10"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="16"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -604,17 +619,17 @@
       <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="13" t="s">
         <v>15</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -636,11 +651,17 @@
       <c r="G3" s="7">
         <v>0.94899999999999995</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="14"/>
+      <c r="H3" s="21">
+        <v>2.9569999999999999</v>
+      </c>
+      <c r="I3" s="22">
+        <v>2.2610000000000001</v>
+      </c>
+      <c r="J3" s="7">
+        <v>1.411</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -656,17 +677,17 @@
       <c r="E4" s="5">
         <v>0.88400000000000001</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="14"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -688,9 +709,9 @@
       <c r="G5" s="8">
         <v>1.752</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="4"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>